<commit_message>
add results of experiment about orthogonal weight and prototype num
</commit_message>
<xml_diff>
--- a/v5/v5_orthogonal/v5_regression_orthogonal_weight.xlsx
+++ b/v5/v5_orthogonal/v5_regression_orthogonal_weight.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wp\Desktop\master\results\analysis_data\standard_orthogonal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\master\ensemble_github\experimental_data\v5\v5_orthogonal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F6EF25A-D0AC-406F-B57C-DF9F9277991E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7DF3024-4A9B-4F37-936B-D71908DE0FBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21840" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -5799,7 +5799,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -6101,17 +6101,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="I147" sqref="I147"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="16" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="27.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.26953125" customWidth="1"/>
+    <col min="2" max="2" width="23.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="16" width="28.54296875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="29.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">

</xml_diff>